<commit_message>
2. atrybuty wszystkie opisane i z funkcjami
</commit_message>
<xml_diff>
--- a/Sprawozdanie_zad2/rys/funkcje.xlsx
+++ b/Sprawozdanie_zad2/rys/funkcje.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xd\inf\6 semestr\Komputerowe systemy rozpoznawania\KSR git\Sprawozdanie_zad2\rys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6AF080-A868-4678-AC06-6ACA9C1B6425}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A0CE19-93FE-421F-BE68-1DA5834F774B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,48 +33,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
-  <si>
-    <t>bardzo młody &amp; 16 &amp; 16 &amp; 18 &amp; 21  \\</t>
-  </si>
-  <si>
-    <t>młody &amp; 20 &amp; 22 &amp; 24 &amp; 25  \\</t>
-  </si>
-  <si>
-    <t>średni &amp; 24 &amp; 26 &amp; 29 &amp; 32  \\</t>
-  </si>
-  <si>
-    <t>bardzo młody</t>
-  </si>
-  <si>
-    <t>młody</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
   <si>
     <t>średni</t>
-  </si>
-  <si>
-    <t>stary</t>
-  </si>
-  <si>
-    <t>niski &amp; 156 &amp; 156 &amp; 166 \\</t>
-  </si>
-  <si>
-    <t>średni &amp; 164 &amp; 170 &amp; 177 \\</t>
-  </si>
-  <si>
-    <t>wysoki &amp; 175 &amp; 182 &amp; 188 \\</t>
-  </si>
-  <si>
-    <t>bardzo wysoki &amp; 186 &amp; 205 &amp; 205  \\</t>
-  </si>
-  <si>
-    <t>niski</t>
-  </si>
-  <si>
-    <t>wysoki</t>
-  </si>
-  <si>
-    <t>bardzo wysoki</t>
   </si>
   <si>
     <t>a</t>
@@ -134,7 +95,46 @@
     <t>gruby</t>
   </si>
   <si>
-    <t xml:space="preserve">stary &amp; 31 &amp; 34 &amp; 42 &amp; 42  </t>
+    <t>słabe</t>
+  </si>
+  <si>
+    <t>średnie</t>
+  </si>
+  <si>
+    <t>dobre</t>
+  </si>
+  <si>
+    <t>bardzo dobre</t>
+  </si>
+  <si>
+    <t>bardzo słabe</t>
+  </si>
+  <si>
+    <t>\item \textsl{(30-60) słabe}</t>
+  </si>
+  <si>
+    <t>\item \textsl{(6-35) bardzo słabe}</t>
+  </si>
+  <si>
+    <t>\item \textsl{(50-70) średnie}</t>
+  </si>
+  <si>
+    <t>\item \textsl{(68-87) dobre}</t>
+  </si>
+  <si>
+    <t>\item \textsl{(85-94) bardzo dobre}</t>
+  </si>
+  <si>
+    <t>słaba</t>
+  </si>
+  <si>
+    <t>średnia</t>
+  </si>
+  <si>
+    <t>duża</t>
+  </si>
+  <si>
+    <t>bardzo duża</t>
   </si>
 </sst>
 </file>
@@ -241,7 +241,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>bardzo młody</c:v>
+                  <c:v>słaba</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -277,16 +277,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -328,7 +328,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>młody</c:v>
+                  <c:v>średnia</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -364,16 +364,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -415,7 +415,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>średni</c:v>
+                  <c:v>duża</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -451,16 +451,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -502,7 +502,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>stary</c:v>
+                  <c:v>bardzo duża</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -538,16 +538,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>31</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100</c:v>
+                  <c:v>888</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -590,13 +590,109 @@
         </c:dLbls>
         <c:axId val="1456754912"/>
         <c:axId val="1385052688"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Arkusz1!$E$9</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent5"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent5"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent5"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Arkusz1!$F$9:$I$9</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="4"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Arkusz1!$F$2:$I$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-4368-4D02-A5FE-FE74125F508D}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="1456754912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="42"/>
-          <c:min val="16"/>
+          <c:max val="95"/>
+          <c:min val="14"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -810,7 +906,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>niski</c:v>
+                  <c:v>bardzo słabe</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -849,10 +945,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>156</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>166</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -891,7 +987,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>średni</c:v>
+                  <c:v>słabe</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -927,13 +1023,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>164</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>170</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>177</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -972,7 +1068,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>wysoki</c:v>
+                  <c:v>średnie</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1008,13 +1104,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>175</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>182</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>188</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1053,7 +1149,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>bardzo wysoki</c:v>
+                  <c:v>dobre</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1089,13 +1185,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>186</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>205</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5000</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1122,6 +1218,87 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-1E3A-46D1-BDBF-001F9105BCDE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$G$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>bardzo dobre</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz1!$H$37:$J$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz1!$H$31:$J$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-621D-48F9-A202-B2835AA86683}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1140,8 +1317,8 @@
         <c:axId val="1453558832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="205"/>
-          <c:min val="156"/>
+          <c:max val="94"/>
+          <c:min val="6"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -4963,15 +5140,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>514349</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>600074</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5334,20 +5511,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:T256"/>
+  <dimension ref="C2:T256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
     <col min="10" max="10" width="9.5703125" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F2">
         <v>0</v>
       </c>
@@ -5361,7 +5539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E3">
         <v>0</v>
       </c>
@@ -5369,106 +5547,86 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5">
+        <v>-15</v>
+      </c>
+      <c r="G5">
         <v>14</v>
       </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>16</v>
-      </c>
       <c r="H5">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="I5">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="F6">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="G6">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="H6">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="I6">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="F7">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="G7">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="H7">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="I7">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="F8">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="G8">
-        <v>34</v>
+        <v>88</v>
       </c>
       <c r="H8">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="I8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="F11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="F13" t="s">
-        <v>33</v>
+        <v>888</v>
       </c>
     </row>
     <row r="31" spans="8:10" x14ac:dyDescent="0.25">
@@ -5484,97 +5642,116 @@
     </row>
     <row r="32" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H32" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="I32" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="J32" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G33" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="H33">
         <v>0</v>
       </c>
       <c r="I33">
-        <v>156</v>
+        <v>6</v>
       </c>
       <c r="J33">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="H34">
-        <v>164</v>
+        <v>20</v>
       </c>
       <c r="I34">
-        <v>170</v>
+        <v>35</v>
       </c>
       <c r="J34">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G35" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="H35">
-        <v>175</v>
+        <v>50</v>
       </c>
       <c r="I35">
-        <v>182</v>
+        <v>60</v>
       </c>
       <c r="J35">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G36" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="H36">
-        <v>186</v>
+        <v>68</v>
       </c>
       <c r="I36">
-        <v>205</v>
+        <v>75</v>
       </c>
       <c r="J36">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E40" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E41" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E42" t="s">
-        <v>10</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>23</v>
+      </c>
+      <c r="H37">
+        <v>85</v>
+      </c>
+      <c r="I37">
+        <v>94</v>
+      </c>
+      <c r="J37">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="49" spans="3:20" x14ac:dyDescent="0.25">
       <c r="F49" s="2" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="3:20" x14ac:dyDescent="0.25">
@@ -5585,25 +5762,25 @@
         <v>2</v>
       </c>
       <c r="J50" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="K50">
         <v>50</v>
       </c>
       <c r="M50" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="N50">
         <v>50</v>
       </c>
       <c r="P50" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="Q50">
         <v>50</v>
       </c>
       <c r="S50" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="T50">
         <v>50</v>
@@ -5611,28 +5788,28 @@
     </row>
     <row r="51" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="J51" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="K51">
         <v>60</v>
       </c>
       <c r="M51" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N51">
         <v>60</v>
       </c>
       <c r="P51" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="Q51">
         <v>60</v>
       </c>
       <c r="S51" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="T51">
         <v>60</v>
@@ -5640,28 +5817,28 @@
     </row>
     <row r="52" spans="3:20" x14ac:dyDescent="0.25">
       <c r="E52" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="J52" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="K52">
         <v>50</v>
       </c>
       <c r="M52" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="N52">
         <v>70</v>
       </c>
       <c r="P52" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q52">
         <v>90</v>
       </c>
       <c r="S52" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="T52">
         <v>110</v>
@@ -5669,32 +5846,32 @@
     </row>
     <row r="53" spans="3:20" x14ac:dyDescent="0.25">
       <c r="E53" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="3"/>
       <c r="J53" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="K53">
         <v>8</v>
       </c>
       <c r="M53" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="N53">
         <v>8</v>
       </c>
       <c r="P53" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="Q53">
         <v>8</v>
       </c>
       <c r="S53" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="T53">
         <v>8</v>
@@ -5702,48 +5879,48 @@
     </row>
     <row r="54" spans="3:20" x14ac:dyDescent="0.25">
       <c r="E54" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="J54" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="K54" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="N54" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="Q54" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T54" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="55" spans="3:20" x14ac:dyDescent="0.25">
       <c r="J55" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="K55" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="M55" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="N55" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="P55" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="Q55" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="S55" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="T55" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="3:20" x14ac:dyDescent="0.25">
@@ -5781,14 +5958,14 @@
         <v>51</v>
       </c>
       <c r="K57" s="2">
-        <f t="shared" ref="K57:K120" si="0">EXP(-((J57-K$52)/K$53)* ((J57-K$52)/K$53))</f>
+        <f t="shared" ref="K57:K116" si="0">EXP(-((J57-K$52)/K$53)* ((J57-K$52)/K$53))</f>
         <v>0.98449643700540845</v>
       </c>
       <c r="M57">
         <v>51</v>
       </c>
       <c r="N57" s="2">
-        <f t="shared" ref="N57:N120" si="1">EXP(-((M57-N$52)/N$53)* ((M57-N$52)/N$53))</f>
+        <f t="shared" ref="N57:N116" si="1">EXP(-((M57-N$52)/N$53)* ((M57-N$52)/N$53))</f>
         <v>3.550648557242539E-3</v>
       </c>
       <c r="P57">

</xml_diff>

<commit_message>
quantifier in class and report
</commit_message>
<xml_diff>
--- a/Sprawozdanie_zad2/rys/funkcje.xlsx
+++ b/Sprawozdanie_zad2/rys/funkcje.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xd\inf\6 semestr\Komputerowe systemy rozpoznawania\KSR git\Sprawozdanie_zad2\rys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A0CE19-93FE-421F-BE68-1DA5834F774B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112837F1-F6A9-465F-A9E9-10F01212141D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
   <si>
     <t>średni</t>
   </si>
@@ -125,16 +125,19 @@
     <t>\item \textsl{(85-94) bardzo dobre}</t>
   </si>
   <si>
-    <t>słaba</t>
+    <t>prawie wszyscy</t>
   </si>
   <si>
-    <t>średnia</t>
+    <t>prawie nikt</t>
   </si>
   <si>
-    <t>duża</t>
+    <t>większość</t>
   </si>
   <si>
-    <t>bardzo duża</t>
+    <t>połowa</t>
+  </si>
+  <si>
+    <t>mniejszość</t>
   </si>
 </sst>
 </file>
@@ -241,7 +244,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>słaba</c:v>
+                  <c:v>prawie nikt</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -277,16 +280,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>-15</c:v>
+                  <c:v>-10000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -328,7 +331,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>średnia</c:v>
+                  <c:v>mniejszość</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -364,16 +367,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>45</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60</c:v>
+                  <c:v>7000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>65</c:v>
+                  <c:v>8000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -415,7 +418,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>duża</c:v>
+                  <c:v>połowa</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -451,16 +454,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>62</c:v>
+                  <c:v>7500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>68</c:v>
+                  <c:v>8000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>80</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>82</c:v>
+                  <c:v>10500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -502,7 +505,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>bardzo duża</c:v>
+                  <c:v>większość</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -538,16 +541,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>80</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>88</c:v>
+                  <c:v>11000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>95</c:v>
+                  <c:v>15000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>888</c:v>
+                  <c:v>16000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -577,6 +580,94 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-8C69-47BC-A4D6-23BF552A3D39}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$E$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>prawie wszyscy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz1!$F$9:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18278</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz1!$F$2:$I$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4368-4D02-A5FE-FE74125F508D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -590,109 +681,14 @@
         </c:dLbls>
         <c:axId val="1456754912"/>
         <c:axId val="1385052688"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredScatterSeries>
-              <c15:ser>
-                <c:idx val="4"/>
-                <c:order val="4"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Arkusz1!$E$9</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="28575" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent5"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent5"/>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent5"/>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:xVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Arkusz1!$F$9:$I$9</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="4"/>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Arkusz1!$F$2:$I$2</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="4"/>
-                      <c:pt idx="0">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>1</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>1</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>0</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="0"/>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000000-4368-4D02-A5FE-FE74125F508D}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredScatterSeries>
-          </c:ext>
-        </c:extLst>
+        <c:extLst/>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="1456754912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="95"/>
-          <c:min val="14"/>
+          <c:max val="18278"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -5140,15 +5136,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
+      <xdr:colOff>609598</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>85724</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>371474</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5514,18 +5510,18 @@
   <dimension ref="C2:T256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
     <col min="10" max="10" width="9.5703125" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:9" x14ac:dyDescent="0.25">
       <c r="F2">
         <v>0</v>
       </c>
@@ -5539,7 +5535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E3">
         <v>0</v>
       </c>
@@ -5547,7 +5543,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:9" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
         <v>1</v>
       </c>
@@ -5561,72 +5557,94 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5">
+        <v>-10000</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>1000</v>
+      </c>
+      <c r="I5">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="6" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6">
+        <v>2000</v>
+      </c>
+      <c r="G6">
+        <v>3000</v>
+      </c>
+      <c r="H6">
+        <v>7000</v>
+      </c>
+      <c r="I6">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7">
+        <v>7500</v>
+      </c>
+      <c r="G7">
+        <v>8000</v>
+      </c>
+      <c r="H7">
+        <v>10000</v>
+      </c>
+      <c r="I7">
+        <v>10500</v>
+      </c>
+    </row>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8">
+        <v>10000</v>
+      </c>
+      <c r="G8">
+        <v>11000</v>
+      </c>
+      <c r="H8">
+        <v>15000</v>
+      </c>
+      <c r="I8">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
         <v>30</v>
       </c>
-      <c r="F5">
-        <v>-15</v>
-      </c>
-      <c r="G5">
-        <v>14</v>
-      </c>
-      <c r="H5">
-        <v>45</v>
-      </c>
-      <c r="I5">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6">
-        <v>45</v>
-      </c>
-      <c r="G6">
-        <v>50</v>
-      </c>
-      <c r="H6">
-        <v>60</v>
-      </c>
-      <c r="I6">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7">
-        <v>62</v>
-      </c>
-      <c r="G7">
-        <v>68</v>
-      </c>
-      <c r="H7">
-        <v>80</v>
-      </c>
-      <c r="I7">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8">
-        <v>80</v>
-      </c>
-      <c r="G8">
-        <v>88</v>
-      </c>
-      <c r="H8">
-        <v>95</v>
-      </c>
-      <c r="I8">
-        <v>888</v>
+      <c r="F9">
+        <v>15000</v>
+      </c>
+      <c r="G9">
+        <v>16500</v>
+      </c>
+      <c r="H9">
+        <v>18278</v>
+      </c>
+      <c r="I9">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>18278</v>
       </c>
     </row>
     <row r="31" spans="8:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
tyd 10 - sprawozdanie, zmiana nazw klas na quantifiers, summarizers
</commit_message>
<xml_diff>
--- a/Sprawozdanie_zad2/rys/funkcje.xlsx
+++ b/Sprawozdanie_zad2/rys/funkcje.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xd\inf\6 semestr\Komputerowe systemy rozpoznawania\KSR git\Sprawozdanie_zad2\rys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112837F1-F6A9-465F-A9E9-10F01212141D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89895F1-7E03-44AC-9B4A-D5591E11D561}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8055" yWindow="4005" windowWidth="14310" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -144,6 +144,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -192,12 +195,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -277,7 +281,7 @@
             <c:numRef>
               <c:f>Arkusz1!$F$5:$I$5</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>-10000</c:v>
@@ -286,10 +290,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>5.4710581026370497E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3000</c:v>
+                  <c:v>0.16413174307911149</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -364,19 +368,19 @@
             <c:numRef>
               <c:f>Arkusz1!$F$6:$I$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2000</c:v>
+                  <c:v>0.10942116205274099</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3000</c:v>
+                  <c:v>0.16413174307911149</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7000</c:v>
+                  <c:v>0.38297406718459348</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8000</c:v>
+                  <c:v>0.43768464821096398</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -451,19 +455,19 @@
             <c:numRef>
               <c:f>Arkusz1!$F$7:$I$7</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7500</c:v>
+                  <c:v>0.41032935769777873</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8000</c:v>
+                  <c:v>0.43768464821096398</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10000</c:v>
+                  <c:v>0.54710581026370497</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10500</c:v>
+                  <c:v>0.57446110077689028</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -538,19 +542,19 @@
             <c:numRef>
               <c:f>Arkusz1!$F$8:$I$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10000</c:v>
+                  <c:v>0.54710581026370497</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11000</c:v>
+                  <c:v>0.60181639129007547</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15000</c:v>
+                  <c:v>0.82065871539555746</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16000</c:v>
+                  <c:v>0.87536929642192796</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -625,16 +629,16 @@
             <c:numRef>
               <c:f>Arkusz1!$F$9:$I$9</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>15000</c:v>
+                  <c:v>0.82065871539555746</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16500</c:v>
+                  <c:v>0.90272458693511326</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18278</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>100000</c:v>
@@ -687,12 +691,12 @@
         <c:axId val="1456754912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="18278"/>
+          <c:max val="1"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5136,15 +5140,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>609598</xdr:colOff>
+      <xdr:colOff>533398</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>371474</xdr:colOff>
+      <xdr:colOff>295274</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5510,13 +5514,16 @@
   <dimension ref="C2:T256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="I9" sqref="F5:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.5703125" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -5561,84 +5568,101 @@
       <c r="E5" t="s">
         <v>31</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="5">
         <v>-10000</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="5">
         <v>0</v>
       </c>
-      <c r="H5">
-        <v>1000</v>
-      </c>
-      <c r="I5">
-        <v>3000</v>
+      <c r="H5" s="5">
+        <f>1000/D12</f>
+        <v>5.4710581026370497E-2</v>
+      </c>
+      <c r="I5" s="5">
+        <f>3000/D12</f>
+        <v>0.16413174307911149</v>
       </c>
     </row>
     <row r="6" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>34</v>
       </c>
-      <c r="F6">
-        <v>2000</v>
-      </c>
-      <c r="G6">
-        <v>3000</v>
-      </c>
-      <c r="H6">
-        <v>7000</v>
-      </c>
-      <c r="I6">
-        <v>8000</v>
+      <c r="F6" s="5">
+        <f>2000/D12</f>
+        <v>0.10942116205274099</v>
+      </c>
+      <c r="G6" s="5">
+        <f>3000/D12</f>
+        <v>0.16413174307911149</v>
+      </c>
+      <c r="H6" s="5">
+        <f>7000/D12</f>
+        <v>0.38297406718459348</v>
+      </c>
+      <c r="I6" s="5">
+        <f>8000/D12</f>
+        <v>0.43768464821096398</v>
       </c>
     </row>
     <row r="7" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
         <v>33</v>
       </c>
-      <c r="F7">
-        <v>7500</v>
-      </c>
-      <c r="G7">
-        <v>8000</v>
-      </c>
-      <c r="H7">
-        <v>10000</v>
-      </c>
-      <c r="I7">
-        <v>10500</v>
+      <c r="F7" s="5">
+        <f>7500/D12</f>
+        <v>0.41032935769777873</v>
+      </c>
+      <c r="G7" s="5">
+        <f>8000/D12</f>
+        <v>0.43768464821096398</v>
+      </c>
+      <c r="H7" s="5">
+        <f>10000/D12</f>
+        <v>0.54710581026370497</v>
+      </c>
+      <c r="I7" s="5">
+        <f>10500/D12</f>
+        <v>0.57446110077689028</v>
       </c>
     </row>
     <row r="8" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>32</v>
       </c>
-      <c r="F8">
-        <v>10000</v>
-      </c>
-      <c r="G8">
-        <v>11000</v>
-      </c>
-      <c r="H8">
-        <v>15000</v>
-      </c>
-      <c r="I8">
-        <v>16000</v>
+      <c r="F8" s="5">
+        <f>10000/D12</f>
+        <v>0.54710581026370497</v>
+      </c>
+      <c r="G8" s="5">
+        <f>11000/D12</f>
+        <v>0.60181639129007547</v>
+      </c>
+      <c r="H8" s="5">
+        <f>15000/D12</f>
+        <v>0.82065871539555746</v>
+      </c>
+      <c r="I8" s="5">
+        <f>16000/D12</f>
+        <v>0.87536929642192796</v>
       </c>
     </row>
     <row r="9" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>30</v>
       </c>
-      <c r="F9">
-        <v>15000</v>
-      </c>
-      <c r="G9">
-        <v>16500</v>
-      </c>
-      <c r="H9">
-        <v>18278</v>
-      </c>
-      <c r="I9">
+      <c r="F9" s="5">
+        <f>15000/D12</f>
+        <v>0.82065871539555746</v>
+      </c>
+      <c r="G9" s="5">
+        <f>16500/D12</f>
+        <v>0.90272458693511326</v>
+      </c>
+      <c r="H9" s="5">
+        <f>18278/D12</f>
+        <v>1</v>
+      </c>
+      <c r="I9" s="5">
         <v>100000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
report sections 1-5, one subject summaries only with relative summarizer
</commit_message>
<xml_diff>
--- a/Sprawozdanie_zad2/rys/funkcje.xlsx
+++ b/Sprawozdanie_zad2/rys/funkcje.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xd\inf\6 semestr\Komputerowe systemy rozpoznawania\KSR git\Sprawozdanie_zad2\rys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89895F1-7E03-44AC-9B4A-D5591E11D561}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5F59C9-0BCB-424E-8C00-29512D8B1954}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8055" yWindow="4005" windowWidth="14310" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -125,29 +125,26 @@
     <t>\item \textsl{(85-94) bardzo dobre}</t>
   </si>
   <si>
-    <t>prawie wszyscy</t>
+    <t>Około 1000</t>
   </si>
   <si>
-    <t>prawie nikt</t>
+    <t>Więcej niż 3000</t>
   </si>
   <si>
-    <t>większość</t>
+    <t>Mniej niż 3000</t>
   </si>
   <si>
-    <t>połowa</t>
+    <t>Około 500</t>
   </si>
   <si>
-    <t>mniejszość</t>
+    <t>Około 100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,6 +164,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC7832"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="3">
@@ -195,13 +206,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -248,7 +268,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>prawie nikt</c:v>
+                  <c:v>Około 1000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -281,19 +301,19 @@
             <c:numRef>
               <c:f>Arkusz1!$F$5:$I$5</c:f>
               <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>-10000</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>960</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.4710581026370497E-2</c:v>
+                  <c:v>1040</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.16413174307911149</c:v>
+                  <c:v>1100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -335,7 +355,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>mniejszość</c:v>
+                  <c:v>Więcej niż 3000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -368,19 +388,19 @@
             <c:numRef>
               <c:f>Arkusz1!$F$6:$I$6</c:f>
               <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.10942116205274099</c:v>
+                  <c:v>2990</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.16413174307911149</c:v>
+                  <c:v>3010</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.38297406718459348</c:v>
+                  <c:v>18278</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.43768464821096398</c:v>
+                  <c:v>18278</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -422,7 +442,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>połowa</c:v>
+                  <c:v>Mniej niż 3000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -455,19 +475,19 @@
             <c:numRef>
               <c:f>Arkusz1!$F$7:$I$7</c:f>
               <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.41032935769777873</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.43768464821096398</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.54710581026370497</c:v>
+                  <c:v>2990</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57446110077689028</c:v>
+                  <c:v>3010</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -509,7 +529,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>większość</c:v>
+                  <c:v>Około 500</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -542,19 +562,19 @@
             <c:numRef>
               <c:f>Arkusz1!$F$8:$I$8</c:f>
               <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.54710581026370497</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.60181639129007547</c:v>
+                  <c:v>480</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.82065871539555746</c:v>
+                  <c:v>520</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.87536929642192796</c:v>
+                  <c:v>550</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -596,7 +616,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>prawie wszyscy</c:v>
+                  <c:v>Około 100</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -629,19 +649,19 @@
             <c:numRef>
               <c:f>Arkusz1!$F$9:$I$9</c:f>
               <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.82065871539555746</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.90272458693511326</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100000</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -691,12 +711,12 @@
         <c:axId val="1456754912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1"/>
+          <c:max val="18278"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5511,19 +5531,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:T256"/>
+  <dimension ref="A2:T256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="F5:I9"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.5703125" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -5566,104 +5586,87 @@
     </row>
     <row r="5" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="5">
-        <v>-10000</v>
+        <v>900</v>
       </c>
       <c r="G5" s="5">
-        <v>0</v>
+        <v>960</v>
       </c>
       <c r="H5" s="5">
-        <f>1000/D12</f>
-        <v>5.4710581026370497E-2</v>
+        <v>1040</v>
       </c>
       <c r="I5" s="5">
-        <f>3000/D12</f>
-        <v>0.16413174307911149</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="6" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F6" s="5">
-        <f>2000/D12</f>
-        <v>0.10942116205274099</v>
+        <v>2990</v>
       </c>
       <c r="G6" s="5">
-        <f>3000/D12</f>
-        <v>0.16413174307911149</v>
+        <v>3010</v>
       </c>
       <c r="H6" s="5">
-        <f>7000/D12</f>
-        <v>0.38297406718459348</v>
+        <v>18278</v>
       </c>
       <c r="I6" s="5">
-        <f>8000/D12</f>
-        <v>0.43768464821096398</v>
+        <v>18278</v>
       </c>
     </row>
     <row r="7" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F7" s="5">
-        <f>7500/D12</f>
-        <v>0.41032935769777873</v>
+        <v>0</v>
       </c>
       <c r="G7" s="5">
-        <f>8000/D12</f>
-        <v>0.43768464821096398</v>
+        <v>0</v>
       </c>
       <c r="H7" s="5">
-        <f>10000/D12</f>
-        <v>0.54710581026370497</v>
+        <v>2990</v>
       </c>
       <c r="I7" s="5">
-        <f>10500/D12</f>
-        <v>0.57446110077689028</v>
+        <v>3010</v>
       </c>
     </row>
     <row r="8" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F8" s="5">
-        <f>10000/D12</f>
-        <v>0.54710581026370497</v>
+        <v>450</v>
       </c>
       <c r="G8" s="5">
-        <f>11000/D12</f>
-        <v>0.60181639129007547</v>
+        <v>480</v>
       </c>
       <c r="H8" s="5">
-        <f>15000/D12</f>
-        <v>0.82065871539555746</v>
+        <v>520</v>
       </c>
       <c r="I8" s="5">
-        <f>16000/D12</f>
-        <v>0.87536929642192796</v>
+        <v>550</v>
       </c>
     </row>
     <row r="9" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F9" s="5">
-        <f>15000/D12</f>
-        <v>0.82065871539555746</v>
+        <v>80</v>
       </c>
       <c r="G9" s="5">
-        <f>16500/D12</f>
-        <v>0.90272458693511326</v>
+        <v>90</v>
       </c>
       <c r="H9" s="5">
-        <f>18278/D12</f>
-        <v>1</v>
+        <v>110</v>
       </c>
       <c r="I9" s="5">
-        <v>100000</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="4:9" x14ac:dyDescent="0.25">
@@ -5671,7 +5674,50 @@
         <v>18278</v>
       </c>
     </row>
-    <row r="31" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="8"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
       <c r="H31">
         <v>0</v>
       </c>
@@ -5682,7 +5728,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
       <c r="H32" t="s">
         <v>1</v>
       </c>
@@ -5693,7 +5740,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
       <c r="G33" t="s">
         <v>24</v>
       </c>
@@ -5707,7 +5755,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="7"/>
       <c r="G34" t="s">
         <v>20</v>
       </c>
@@ -5721,7 +5770,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
       <c r="G35" t="s">
         <v>21</v>
       </c>
@@ -5735,7 +5785,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G36" t="s">
         <v>22</v>
       </c>
@@ -5749,7 +5799,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
         <v>23</v>
       </c>
@@ -5763,27 +5813,27 @@
         <v>150</v>
       </c>
     </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
         <v>29</v>
       </c>

</xml_diff>